<commit_message>
Update error processing and report generation scripts
Improved user path handling in report generation, added support for Integratour data, and refined responsibility allocation logic for ZUPPER and KONTRIP in error processing. Also removed unused Benner support allocation and updated several Excel and PDF report files, including adding a new ZUPPER VIAGENS report.
</commit_message>
<xml_diff>
--- a/Integration Quality/EMPRESAS/Relatorio - KONTRIP VIAGENS.xlsx
+++ b/Integration Quality/EMPRESAS/Relatorio - KONTRIP VIAGENS.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ16"/>
+  <dimension ref="A1:AQ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,59 +700,59 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="n">
-        <v>22443138</v>
+        <v>22461262</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>23286164</v>
+        <v>23300940</v>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>ACC</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D2" s="6" t="n">
-        <v>45831.58079861111</v>
+        <v>45834.70292824074</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>45831.58729166666</v>
+        <v>45834.70704861111</v>
       </c>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>QZUVKB</t>
+          <t>GMPQBQ</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J2" s="5" t="inlineStr">
         <is>
-          <t>ALDA MARINA DE CAMPOS MELO</t>
+          <t>DA SILVA CASTRO/VICTOR</t>
         </is>
       </c>
       <c r="K2" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L2" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M2" s="6" t="n">
-        <v>45828.58055555556</v>
+        <v>45834.69861111111</v>
       </c>
       <c r="N2" s="5" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
       </c>
       <c r="V2" s="5" t="inlineStr">
         <is>
-          <t>Vpr Consultoria, Eventos, Servicos e Treinamentos Ltda</t>
+          <t>Pessoa e Pessoa Advogados Associados</t>
         </is>
       </c>
       <c r="W2" s="5" t="inlineStr">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="Y2" s="5" t="n">
-        <v>2139988704</v>
+        <v>2140277329</v>
       </c>
       <c r="Z2" s="5" t="inlineStr">
         <is>
@@ -823,10 +823,10 @@
         </is>
       </c>
       <c r="AB2" s="5" t="n">
-        <v>2015.77</v>
+        <v>1191.9</v>
       </c>
       <c r="AC2" s="5" t="n">
-        <v>59.95</v>
+        <v>104.89</v>
       </c>
       <c r="AD2" s="5" t="n">
         <v>0</v>
@@ -841,16 +841,16 @@
         <v>0</v>
       </c>
       <c r="AH2" s="5" t="n">
-        <v>120.95</v>
+        <v>71.51000000000001</v>
       </c>
       <c r="AI2" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ2" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>Centro de custo não preenchido! (ACC01)</t>
         </is>
       </c>
       <c r="AK2" s="5" t="inlineStr">
@@ -860,17 +860,17 @@
       </c>
       <c r="AL2" s="5" t="inlineStr">
         <is>
+          <t>Centro de custo</t>
+        </is>
+      </c>
+      <c r="AM2" s="5" t="inlineStr">
+        <is>
           <t>Falta de informação Gerencial</t>
         </is>
       </c>
-      <c r="AM2" s="5" t="inlineStr">
-        <is>
-          <t>Rateio de centro de custo/projeto</t>
-        </is>
-      </c>
       <c r="AN2" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Dados do Fornecedor</t>
         </is>
       </c>
       <c r="AO2" s="5" t="inlineStr">
@@ -891,10 +891,10 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="n">
-        <v>22443418</v>
+        <v>22459992</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>23286368</v>
+        <v>23299710</v>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
@@ -902,24 +902,24 @@
         </is>
       </c>
       <c r="D3" s="6" t="n">
-        <v>45831.61105324074</v>
+        <v>45834.52964120371</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>45831.61527777778</v>
+        <v>45834.73059027778</v>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>HRTRXM</t>
+          <t>LA9571600AUXS</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="J3" s="5" t="inlineStr">
         <is>
-          <t>SILVIO CRESPO</t>
+          <t>VALERIA GOMES LEAL</t>
         </is>
       </c>
       <c r="K3" s="5" t="inlineStr">
@@ -943,7 +943,7 @@
         </is>
       </c>
       <c r="M3" s="6" t="n">
-        <v>45828.61041666667</v>
+        <v>45833.52916666667</v>
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
@@ -962,12 +962,12 @@
       </c>
       <c r="Q3" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Invoice</t>
         </is>
       </c>
       <c r="R3" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Cartão convênio</t>
         </is>
       </c>
       <c r="S3" s="5" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="V3" s="5" t="inlineStr">
         <is>
-          <t>Grana Capital Tecnologia Em Investimentos Ltda</t>
+          <t>Kontrip - Vendas Cartao de Credito</t>
         </is>
       </c>
       <c r="W3" s="5" t="inlineStr">
@@ -997,11 +997,11 @@
       </c>
       <c r="X3" s="5" t="inlineStr">
         <is>
-          <t>Gol Linhas Aereas</t>
+          <t>Latam Airlines Brasil</t>
         </is>
       </c>
       <c r="Y3" s="5" t="n">
-        <v>2139949448</v>
+        <v>2238480836</v>
       </c>
       <c r="Z3" s="5" t="inlineStr">
         <is>
@@ -1014,10 +1014,10 @@
         </is>
       </c>
       <c r="AB3" s="5" t="n">
-        <v>198.7</v>
+        <v>1785.44</v>
       </c>
       <c r="AC3" s="5" t="n">
-        <v>34.11</v>
+        <v>78.38</v>
       </c>
       <c r="AD3" s="5" t="n">
         <v>0</v>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="AH3" s="5" t="n">
-        <v>11.92</v>
+        <v>30.53</v>
       </c>
       <c r="AI3" s="5" t="inlineStr">
         <is>
@@ -1082,59 +1082,59 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="n">
-        <v>22443698</v>
+        <v>22460028</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>23286625</v>
+        <v>23299735</v>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC</t>
         </is>
       </c>
       <c r="D4" s="6" t="n">
-        <v>45831.63736111111</v>
+        <v>45834.53344907407</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>45831.63805555556</v>
+        <v>45834.73065972222</v>
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
-          <t>UGDCFT</t>
+          <t>LA9577150CBWZ</t>
         </is>
       </c>
       <c r="I4" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J4" s="5" t="inlineStr">
         <is>
-          <t>FERNANDES/DANIEL</t>
+          <t>FRANCISCO CANINDE FERNANDES JUNIOR</t>
         </is>
       </c>
       <c r="K4" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M4" s="6" t="n">
-        <v>45831.59166666667</v>
+        <v>45833.53333333333</v>
       </c>
       <c r="N4" s="5" t="inlineStr">
         <is>
@@ -1153,12 +1153,12 @@
       </c>
       <c r="Q4" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Invoice</t>
         </is>
       </c>
       <c r="R4" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Cartão convênio</t>
         </is>
       </c>
       <c r="S4" s="5" t="inlineStr">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="U4" s="5" t="inlineStr">
         <is>
-          <t>Independente</t>
+          <t>Grupo Kontrip</t>
         </is>
       </c>
       <c r="V4" s="5" t="inlineStr">
         <is>
-          <t>Tap Air Portugal</t>
+          <t>Nossa Engenharia e Servicos</t>
         </is>
       </c>
       <c r="W4" s="5" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="X4" s="5" t="inlineStr">
         <is>
-          <t>Gol Linhas Aereas</t>
+          <t>Latam Airlines Brasil</t>
         </is>
       </c>
       <c r="Y4" s="5" t="n">
-        <v>2140079741</v>
+        <v>2238555012</v>
       </c>
       <c r="Z4" s="5" t="inlineStr">
         <is>
@@ -1205,10 +1205,10 @@
         </is>
       </c>
       <c r="AB4" s="5" t="n">
-        <v>928.1</v>
+        <v>1199.69</v>
       </c>
       <c r="AC4" s="5" t="n">
-        <v>50.92</v>
+        <v>102.22</v>
       </c>
       <c r="AD4" s="5" t="n">
         <v>0</v>
@@ -1223,16 +1223,16 @@
         <v>0</v>
       </c>
       <c r="AH4" s="5" t="n">
-        <v>55.69</v>
+        <v>20.51</v>
       </c>
       <c r="AI4" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ4" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo não preenchido! (ACC01)</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK4" s="5" t="inlineStr">
@@ -1242,17 +1242,17 @@
       </c>
       <c r="AL4" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM4" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN4" s="5" t="inlineStr">
         <is>
-          <t>Dados do Fornecedor</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO4" s="5" t="inlineStr">
@@ -1273,59 +1273,59 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="n">
-        <v>22443998</v>
+        <v>22459944</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>23286896</v>
+        <v>23299686</v>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC</t>
         </is>
       </c>
       <c r="D5" s="6" t="n">
-        <v>45831.67209490741</v>
+        <v>45834.52306712963</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>45831.67363425926</v>
+        <v>45834.73011574074</v>
       </c>
       <c r="F5" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
-          <t>LA9574694UPEM</t>
+          <t>LA9572362DNZW</t>
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J5" s="5" t="inlineStr">
         <is>
-          <t>rui pinhal/mario</t>
+          <t>CAIO FABIO ALVES CASTRO</t>
         </is>
       </c>
       <c r="K5" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M5" s="6" t="n">
-        <v>45831.59652777778</v>
+        <v>45833.52291666667</v>
       </c>
       <c r="N5" s="5" t="inlineStr">
         <is>
@@ -1344,12 +1344,12 @@
       </c>
       <c r="Q5" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Invoice</t>
         </is>
       </c>
       <c r="R5" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Cartão convênio</t>
         </is>
       </c>
       <c r="S5" s="5" t="inlineStr">
@@ -1364,12 +1364,12 @@
       </c>
       <c r="U5" s="5" t="inlineStr">
         <is>
-          <t>Independente</t>
+          <t>Grupo Kontrip</t>
         </is>
       </c>
       <c r="V5" s="5" t="inlineStr">
         <is>
-          <t>Tap Air Portugal</t>
+          <t>Marques e Bezerra Ltda</t>
         </is>
       </c>
       <c r="W5" s="5" t="inlineStr">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="Y5" s="5" t="n">
-        <v>2238221759</v>
+        <v>2238457649</v>
       </c>
       <c r="Z5" s="5" t="inlineStr">
         <is>
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="AB5" s="5" t="n">
-        <v>919.11</v>
+        <v>1608.04</v>
       </c>
       <c r="AC5" s="5" t="n">
-        <v>82.36</v>
+        <v>95.34</v>
       </c>
       <c r="AD5" s="5" t="n">
         <v>0</v>
@@ -1414,16 +1414,16 @@
         <v>0</v>
       </c>
       <c r="AH5" s="5" t="n">
-        <v>13.79</v>
+        <v>27.5</v>
       </c>
       <c r="AI5" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ5" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo não preenchido! (ACC01)</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK5" s="5" t="inlineStr">
@@ -1433,17 +1433,17 @@
       </c>
       <c r="AL5" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM5" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN5" s="5" t="inlineStr">
         <is>
-          <t>Dados do Fornecedor</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO5" s="5" t="inlineStr">
@@ -1464,10 +1464,10 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="n">
-        <v>22442897</v>
+        <v>22459872</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>23285884</v>
+        <v>23299568</v>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
@@ -1475,48 +1475,48 @@
         </is>
       </c>
       <c r="D6" s="6" t="n">
-        <v>45831.55122685185</v>
+        <v>45834.51140046296</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>45831.55306712963</v>
+        <v>45834.72637731482</v>
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
-          <t>FDUEIN</t>
+          <t>SF3F6L</t>
         </is>
       </c>
       <c r="I6" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J6" s="5" t="inlineStr">
         <is>
-          <t>Ribeiro Guth/Alberto</t>
+          <t>CAMILA DO NASCIMENTO CAMPOS KAERCHER</t>
         </is>
       </c>
       <c r="K6" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M6" s="6" t="n">
-        <v>45831.54930555556</v>
+        <v>45833.51111111111</v>
       </c>
       <c r="N6" s="5" t="inlineStr">
         <is>
@@ -1560,7 +1560,7 @@
       </c>
       <c r="V6" s="5" t="inlineStr">
         <is>
-          <t>Matterhorn Infraestrutura Gestao de Investimentos Ltda</t>
+          <t>Kaercher Treinamentos</t>
         </is>
       </c>
       <c r="W6" s="5" t="inlineStr">
@@ -1570,11 +1570,11 @@
       </c>
       <c r="X6" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y6" s="5" t="n">
-        <v>2238191518</v>
+        <v>3023299567</v>
       </c>
       <c r="Z6" s="5" t="inlineStr">
         <is>
@@ -1587,10 +1587,10 @@
         </is>
       </c>
       <c r="AB6" s="5" t="n">
-        <v>2498.21</v>
+        <v>1751.51</v>
       </c>
       <c r="AC6" s="5" t="n">
-        <v>289.52</v>
+        <v>74.59</v>
       </c>
       <c r="AD6" s="5" t="n">
         <v>0</v>
@@ -1605,16 +1605,16 @@
         <v>0</v>
       </c>
       <c r="AH6" s="5" t="n">
-        <v>40</v>
+        <v>472.91</v>
       </c>
       <c r="AI6" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ6" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo não preenchido! (ACC01) Solicitante não preenchido! (ACC01)</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK6" s="5" t="inlineStr">
@@ -1624,17 +1624,17 @@
       </c>
       <c r="AL6" s="5" t="inlineStr">
         <is>
-          <t>Mais de um campo não preenchido</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM6" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN6" s="5" t="inlineStr">
         <is>
-          <t>Dados do Fornecedor</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO6" s="5" t="inlineStr">
@@ -1655,59 +1655,59 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="n">
-        <v>22443137</v>
+        <v>22459872</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>23286108</v>
+        <v>23299589</v>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC02</t>
         </is>
       </c>
       <c r="D7" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.51140046296</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.72637731482</v>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>SF3F6L</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
-          <t>ARAUJO/BENITO</t>
+          <t>MARIANA CERQUEIRA DE ALMEIDA</t>
         </is>
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M7" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45833.51111111111</v>
       </c>
       <c r="N7" s="5" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="V7" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Kaercher Treinamentos</t>
         </is>
       </c>
       <c r="W7" s="5" t="inlineStr">
@@ -1761,11 +1761,11 @@
       </c>
       <c r="X7" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y7" s="5" t="n">
-        <v>2238198211</v>
+        <v>3023299591</v>
       </c>
       <c r="Z7" s="5" t="inlineStr">
         <is>
@@ -1778,10 +1778,10 @@
         </is>
       </c>
       <c r="AB7" s="5" t="n">
-        <v>1161.19</v>
+        <v>1751.51</v>
       </c>
       <c r="AC7" s="5" t="n">
-        <v>48.16</v>
+        <v>74.59</v>
       </c>
       <c r="AD7" s="5" t="n">
         <v>0</v>
@@ -1796,16 +1796,16 @@
         <v>0</v>
       </c>
       <c r="AH7" s="5" t="n">
-        <v>487.71</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ7" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK7" s="5" t="inlineStr">
@@ -1815,17 +1815,17 @@
       </c>
       <c r="AL7" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM7" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN7" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO7" s="5" t="inlineStr">
@@ -1840,65 +1840,65 @@
       </c>
       <c r="AQ7" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="n">
-        <v>22443137</v>
+        <v>22459872</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>23286109</v>
+        <v>23299595</v>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>ACC02</t>
+          <t>ACC03</t>
         </is>
       </c>
       <c r="D8" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.51140046296</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.72637731482</v>
       </c>
       <c r="F8" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G8" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H8" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>SF3F6L</t>
         </is>
       </c>
       <c r="I8" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J8" s="5" t="inlineStr">
         <is>
-          <t>SILVA/SUELLEN</t>
+          <t>LUCAS GONCALVES GOMES SILVA</t>
         </is>
       </c>
       <c r="K8" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L8" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M8" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45833.51111111111</v>
       </c>
       <c r="N8" s="5" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="V8" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Kaercher Treinamentos</t>
         </is>
       </c>
       <c r="W8" s="5" t="inlineStr">
@@ -1952,11 +1952,11 @@
       </c>
       <c r="X8" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y8" s="5" t="n">
-        <v>2238198212</v>
+        <v>3023299596</v>
       </c>
       <c r="Z8" s="5" t="inlineStr">
         <is>
@@ -1969,10 +1969,10 @@
         </is>
       </c>
       <c r="AB8" s="5" t="n">
-        <v>1161.22</v>
+        <v>1751.51</v>
       </c>
       <c r="AC8" s="5" t="n">
-        <v>48.16</v>
+        <v>74.59</v>
       </c>
       <c r="AD8" s="5" t="n">
         <v>0</v>
@@ -1991,12 +1991,12 @@
       </c>
       <c r="AI8" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ8" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK8" s="5" t="inlineStr">
@@ -2006,17 +2006,17 @@
       </c>
       <c r="AL8" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM8" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN8" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO8" s="5" t="inlineStr">
@@ -2031,41 +2031,41 @@
       </c>
       <c r="AQ8" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="n">
-        <v>22443137</v>
+        <v>22459937</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>23286110</v>
+        <v>23299646</v>
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>ACC03</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D9" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.52216435185</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.52375</v>
       </c>
       <c r="F9" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G9" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H9" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>XNRYUD</t>
         </is>
       </c>
       <c r="I9" s="5" t="inlineStr">
@@ -2075,7 +2075,7 @@
       </c>
       <c r="J9" s="5" t="inlineStr">
         <is>
-          <t>Marques/Jonnata</t>
+          <t>DE ARRUDA QUINTEIRO/BRUNNA</t>
         </is>
       </c>
       <c r="K9" s="5" t="inlineStr">
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="M9" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45834.52152777778</v>
       </c>
       <c r="N9" s="5" t="inlineStr">
         <is>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="V9" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Kontrip - Vendas Cartao de Credito</t>
         </is>
       </c>
       <c r="W9" s="5" t="inlineStr">
@@ -2143,11 +2143,11 @@
       </c>
       <c r="X9" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y9" s="5" t="n">
-        <v>2238198213</v>
+        <v>496701246</v>
       </c>
       <c r="Z9" s="5" t="inlineStr">
         <is>
@@ -2160,10 +2160,10 @@
         </is>
       </c>
       <c r="AB9" s="5" t="n">
-        <v>1161.22</v>
+        <v>2089.19</v>
       </c>
       <c r="AC9" s="5" t="n">
-        <v>48.16</v>
+        <v>450</v>
       </c>
       <c r="AD9" s="5" t="n">
         <v>0</v>
@@ -2178,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="AH9" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AI9" s="5" t="inlineStr">
         <is>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="AJ9" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
         </is>
       </c>
       <c r="AK9" s="5" t="inlineStr">
@@ -2197,12 +2197,12 @@
       </c>
       <c r="AL9" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Duplicidade de RLOC</t>
         </is>
       </c>
       <c r="AM9" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Campo RLOC</t>
         </is>
       </c>
       <c r="AN9" s="5" t="inlineStr">
@@ -2222,41 +2222,41 @@
       </c>
       <c r="AQ9" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="n">
-        <v>22443137</v>
+        <v>22461196</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>23286111</v>
+        <v>23300868</v>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>ACC04</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D10" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.69434027778</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.69774305556</v>
       </c>
       <c r="F10" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G10" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H10" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>NJZS5M</t>
         </is>
       </c>
       <c r="I10" s="5" t="inlineStr">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="J10" s="5" t="inlineStr">
         <is>
-          <t>JANUARIO/BRUNO</t>
+          <t>Varalda/Adriana</t>
         </is>
       </c>
       <c r="K10" s="5" t="inlineStr">
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="M10" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45834.67777777778</v>
       </c>
       <c r="N10" s="5" t="inlineStr">
         <is>
@@ -2324,7 +2324,7 @@
       </c>
       <c r="V10" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Kontrip - Vendas Cartao de Credito</t>
         </is>
       </c>
       <c r="W10" s="5" t="inlineStr">
@@ -2334,11 +2334,11 @@
       </c>
       <c r="X10" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y10" s="5" t="n">
-        <v>2238198214</v>
+        <v>119583055</v>
       </c>
       <c r="Z10" s="5" t="inlineStr">
         <is>
@@ -2351,10 +2351,10 @@
         </is>
       </c>
       <c r="AB10" s="5" t="n">
-        <v>1161.22</v>
+        <v>1790</v>
       </c>
       <c r="AC10" s="5" t="n">
-        <v>48.16</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="5" t="n">
         <v>0</v>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="AH10" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AI10" s="5" t="inlineStr">
         <is>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AJ10" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
         </is>
       </c>
       <c r="AK10" s="5" t="inlineStr">
@@ -2388,12 +2388,12 @@
       </c>
       <c r="AL10" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Duplicidade de RLOC</t>
         </is>
       </c>
       <c r="AM10" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Campo RLOC</t>
         </is>
       </c>
       <c r="AN10" s="5" t="inlineStr">
@@ -2413,65 +2413,65 @@
       </c>
       <c r="AQ10" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="n">
-        <v>22443137</v>
+        <v>22459821</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>23286112</v>
+        <v>23299526</v>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>ACC05</t>
+          <t>ACC</t>
         </is>
       </c>
       <c r="D11" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.50327546296</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.70680555556</v>
       </c>
       <c r="F11" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G11" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H11" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>RK8PPM</t>
         </is>
       </c>
       <c r="I11" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J11" s="5" t="inlineStr">
         <is>
-          <t>ALBINO/GUSTAVO</t>
+          <t>THIAGO DE LIMA FAUSTINO</t>
         </is>
       </c>
       <c r="K11" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L11" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M11" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45833.50277777778</v>
       </c>
       <c r="N11" s="5" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="V11" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Kontrip - Vendas Cartao de Credito</t>
         </is>
       </c>
       <c r="W11" s="5" t="inlineStr">
@@ -2525,11 +2525,11 @@
       </c>
       <c r="X11" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y11" s="5" t="n">
-        <v>2238198215</v>
+        <v>3023299525</v>
       </c>
       <c r="Z11" s="5" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="AB11" s="5" t="n">
-        <v>1161.22</v>
+        <v>1058.92</v>
       </c>
       <c r="AC11" s="5" t="n">
-        <v>48.16</v>
+        <v>34.11</v>
       </c>
       <c r="AD11" s="5" t="n">
         <v>0</v>
@@ -2560,16 +2560,16 @@
         <v>0</v>
       </c>
       <c r="AH11" s="5" t="n">
-        <v>0</v>
+        <v>95.3</v>
       </c>
       <c r="AI11" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ11" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK11" s="5" t="inlineStr">
@@ -2579,17 +2579,17 @@
       </c>
       <c r="AL11" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM11" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN11" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO11" s="5" t="inlineStr">
@@ -2604,65 +2604,65 @@
       </c>
       <c r="AQ11" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="n">
-        <v>22443137</v>
+        <v>22460105</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>23286113</v>
+        <v>23299810</v>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>ACC06</t>
+          <t>ACC</t>
         </is>
       </c>
       <c r="D12" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.54712962963</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.72902777778</v>
       </c>
       <c r="F12" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H12" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>JHS6PS</t>
         </is>
       </c>
       <c r="I12" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J12" s="5" t="inlineStr">
         <is>
-          <t>CAMARGO/JULIANA</t>
+          <t>CAROLINE CELLI</t>
         </is>
       </c>
       <c r="K12" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L12" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M12" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45833.54652777778</v>
       </c>
       <c r="N12" s="5" t="inlineStr">
         <is>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="V12" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Mauro Goncalve Antonelli</t>
         </is>
       </c>
       <c r="W12" s="5" t="inlineStr">
@@ -2716,11 +2716,11 @@
       </c>
       <c r="X12" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y12" s="5" t="n">
-        <v>2238198216</v>
+        <v>3023299809</v>
       </c>
       <c r="Z12" s="5" t="inlineStr">
         <is>
@@ -2733,10 +2733,10 @@
         </is>
       </c>
       <c r="AB12" s="5" t="n">
-        <v>1161.22</v>
+        <v>1574.88</v>
       </c>
       <c r="AC12" s="5" t="n">
-        <v>48.16</v>
+        <v>46.72</v>
       </c>
       <c r="AD12" s="5" t="n">
         <v>0</v>
@@ -2751,16 +2751,16 @@
         <v>0</v>
       </c>
       <c r="AH12" s="5" t="n">
-        <v>0</v>
+        <v>141.74</v>
       </c>
       <c r="AI12" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ12" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK12" s="5" t="inlineStr">
@@ -2770,17 +2770,17 @@
       </c>
       <c r="AL12" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM12" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN12" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO12" s="5" t="inlineStr">
@@ -2795,65 +2795,65 @@
       </c>
       <c r="AQ12" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="n">
-        <v>22443137</v>
+        <v>22459766</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>23286114</v>
+        <v>23299457</v>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>ACC07</t>
+          <t>ACC</t>
         </is>
       </c>
       <c r="D13" s="6" t="n">
-        <v>45831.58091435185</v>
+        <v>45834.49883101852</v>
       </c>
       <c r="E13" s="6" t="n">
-        <v>45831.58263888889</v>
+        <v>45834.70751157407</v>
       </c>
       <c r="F13" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G13" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H13" s="5" t="inlineStr">
         <is>
-          <t>LA9577948KSFD</t>
+          <t>GRS1HB</t>
         </is>
       </c>
       <c r="I13" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J13" s="5" t="inlineStr">
         <is>
-          <t>RACHINSKI/RAFAEL</t>
+          <t>SAMUEL SILVA</t>
         </is>
       </c>
       <c r="K13" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L13" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M13" s="6" t="n">
-        <v>45831.43680555555</v>
+        <v>45833.49861111111</v>
       </c>
       <c r="N13" s="5" t="inlineStr">
         <is>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="V13" s="5" t="inlineStr">
         <is>
-          <t>Associacao Colo de Deus e Santissima Virgem (a.c.d.s.v)</t>
+          <t>Galzer Importacao e Exportacao Ltda</t>
         </is>
       </c>
       <c r="W13" s="5" t="inlineStr">
@@ -2907,11 +2907,11 @@
       </c>
       <c r="X13" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y13" s="5" t="n">
-        <v>2238198216</v>
+        <v>3023299456</v>
       </c>
       <c r="Z13" s="5" t="inlineStr">
         <is>
@@ -2924,10 +2924,10 @@
         </is>
       </c>
       <c r="AB13" s="5" t="n">
-        <v>1161.22</v>
+        <v>227.84</v>
       </c>
       <c r="AC13" s="5" t="n">
-        <v>48.16</v>
+        <v>65</v>
       </c>
       <c r="AD13" s="5" t="n">
         <v>0</v>
@@ -2942,16 +2942,16 @@
         <v>0</v>
       </c>
       <c r="AH13" s="5" t="n">
-        <v>0</v>
+        <v>20.51</v>
       </c>
       <c r="AI13" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ13" s="5" t="inlineStr">
         <is>
-          <t>Verificação de bilhetes: Bilhete 2238198216 já sendo utilizado para este fornecedor.</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK13" s="5" t="inlineStr">
@@ -2961,17 +2961,17 @@
       </c>
       <c r="AL13" s="5" t="inlineStr">
         <is>
-          <t>Bilhete duplicado</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM13" s="5" t="inlineStr">
         <is>
-          <t>Bilhete Já Contabilizado</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN13" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO13" s="5" t="inlineStr">
@@ -2986,65 +2986,65 @@
       </c>
       <c r="AQ13" s="5" t="inlineStr">
         <is>
-          <t>Conciliação aérea</t>
+          <t>Operações - KONTRIP</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="n">
-        <v>22444419</v>
+        <v>22459866</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>23287293</v>
+        <v>23299554</v>
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC</t>
         </is>
       </c>
       <c r="D14" s="6" t="n">
-        <v>45831.72347222222</v>
+        <v>45834.50763888889</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>45831.72582175926</v>
+        <v>45834.72603009259</v>
       </c>
       <c r="F14" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="G14" s="5" t="inlineStr">
         <is>
-          <t>0 a 02 dias</t>
+          <t>03 a 05 dias</t>
         </is>
       </c>
       <c r="H14" s="5" t="inlineStr">
         <is>
-          <t>LA9571170HTTN</t>
+          <t>GLBGMG</t>
         </is>
       </c>
       <c r="I14" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J14" s="5" t="inlineStr">
         <is>
-          <t>Alves Magalhães Filho/Jorge</t>
+          <t>CHARLLES RODRIGUES</t>
         </is>
       </c>
       <c r="K14" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L14" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M14" s="6" t="n">
-        <v>45831.72222222222</v>
+        <v>45833.50763888889</v>
       </c>
       <c r="N14" s="5" t="inlineStr">
         <is>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="V14" s="5" t="inlineStr">
         <is>
-          <t>Lmaismaocubo Projetos e Consultoria Ltda</t>
+          <t>Galzer Importacao e Exportacao Ltda</t>
         </is>
       </c>
       <c r="W14" s="5" t="inlineStr">
@@ -3098,11 +3098,11 @@
       </c>
       <c r="X14" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Azul Linhas Aereas</t>
         </is>
       </c>
       <c r="Y14" s="5" t="n">
-        <v>2238234777</v>
+        <v>3023299553</v>
       </c>
       <c r="Z14" s="5" t="inlineStr">
         <is>
@@ -3115,10 +3115,10 @@
         </is>
       </c>
       <c r="AB14" s="5" t="n">
-        <v>419.02</v>
+        <v>232.34</v>
       </c>
       <c r="AC14" s="5" t="n">
-        <v>100.18</v>
+        <v>65</v>
       </c>
       <c r="AD14" s="5" t="n">
         <v>0</v>
@@ -3133,16 +3133,16 @@
         <v>0</v>
       </c>
       <c r="AH14" s="5" t="n">
-        <v>40</v>
+        <v>20.91</v>
       </c>
       <c r="AI14" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ14" s="5" t="inlineStr">
         <is>
-          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK14" s="5" t="inlineStr">
@@ -3152,17 +3152,17 @@
       </c>
       <c r="AL14" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de RLOC</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM14" s="5" t="inlineStr">
         <is>
-          <t>Campo RLOC</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN14" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO14" s="5" t="inlineStr">
@@ -3176,388 +3176,6 @@
         </is>
       </c>
       <c r="AQ14" s="5" t="inlineStr">
-        <is>
-          <t>Conciliação aérea</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n">
-        <v>22442491</v>
-      </c>
-      <c r="B15" s="5" t="n">
-        <v>23285512</v>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>ACC01</t>
-        </is>
-      </c>
-      <c r="D15" s="6" t="n">
-        <v>45831.50450231481</v>
-      </c>
-      <c r="E15" s="6" t="n">
-        <v>45831.51125</v>
-      </c>
-      <c r="F15" s="5" t="inlineStr">
-        <is>
-          <t>0 a 02 dias</t>
-        </is>
-      </c>
-      <c r="G15" s="5" t="inlineStr">
-        <is>
-          <t>0 a 02 dias</t>
-        </is>
-      </c>
-      <c r="H15" s="5" t="inlineStr">
-        <is>
-          <t>OG584V</t>
-        </is>
-      </c>
-      <c r="I15" s="5" t="inlineStr">
-        <is>
-          <t>MANUAL</t>
-        </is>
-      </c>
-      <c r="J15" s="5" t="inlineStr">
-        <is>
-          <t>DAVI ARAUJO</t>
-        </is>
-      </c>
-      <c r="K15" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="L15" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="M15" s="6" t="n">
-        <v>45828.50416666667</v>
-      </c>
-      <c r="N15" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O15" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P15" s="5" t="inlineStr">
-        <is>
-          <t>OFF LINE</t>
-        </is>
-      </c>
-      <c r="Q15" s="5" t="inlineStr">
-        <is>
-          <t>Invoice</t>
-        </is>
-      </c>
-      <c r="R15" s="5" t="inlineStr">
-        <is>
-          <t>Cartão convênio</t>
-        </is>
-      </c>
-      <c r="S15" s="5" t="inlineStr">
-        <is>
-          <t>Aéreo</t>
-        </is>
-      </c>
-      <c r="T15" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="U15" s="5" t="inlineStr">
-        <is>
-          <t>Grupo Kontrip</t>
-        </is>
-      </c>
-      <c r="V15" s="5" t="inlineStr">
-        <is>
-          <t>Porto de Galinhas Convention e Visitors Bureau</t>
-        </is>
-      </c>
-      <c r="W15" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X15" s="5" t="inlineStr">
-        <is>
-          <t>Azul Linhas Aereas</t>
-        </is>
-      </c>
-      <c r="Y15" s="5" t="n">
-        <v>3023285511</v>
-      </c>
-      <c r="Z15" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AA15" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB15" s="5" t="n">
-        <v>612.54</v>
-      </c>
-      <c r="AC15" s="5" t="n">
-        <v>119.51</v>
-      </c>
-      <c r="AD15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="5" t="n">
-        <v>110.26</v>
-      </c>
-      <c r="AI15" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ15" s="5" t="inlineStr">
-        <is>
-          <t>36Faltou informar rateio de centro de custo/projeto abaixo da accounting</t>
-        </is>
-      </c>
-      <c r="AK15" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AL15" s="5" t="inlineStr">
-        <is>
-          <t>Falta de informação Gerencial</t>
-        </is>
-      </c>
-      <c r="AM15" s="5" t="inlineStr">
-        <is>
-          <t>Rateio de centro de custo/projeto</t>
-        </is>
-      </c>
-      <c r="AN15" s="5" t="inlineStr">
-        <is>
-          <t>Dados Gerenciais</t>
-        </is>
-      </c>
-      <c r="AO15" s="5" t="inlineStr">
-        <is>
-          <t>Qualidade dos dados</t>
-        </is>
-      </c>
-      <c r="AP15" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP VIAGENS</t>
-        </is>
-      </c>
-      <c r="AQ15" s="5" t="inlineStr">
-        <is>
-          <t>Operações - KONTRIP</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="n">
-        <v>22442491</v>
-      </c>
-      <c r="B16" s="5" t="n">
-        <v>23285535</v>
-      </c>
-      <c r="C16" s="5" t="inlineStr">
-        <is>
-          <t>ACC02</t>
-        </is>
-      </c>
-      <c r="D16" s="6" t="n">
-        <v>45831.50450231481</v>
-      </c>
-      <c r="E16" s="6" t="n">
-        <v>45831.51125</v>
-      </c>
-      <c r="F16" s="5" t="inlineStr">
-        <is>
-          <t>0 a 02 dias</t>
-        </is>
-      </c>
-      <c r="G16" s="5" t="inlineStr">
-        <is>
-          <t>0 a 02 dias</t>
-        </is>
-      </c>
-      <c r="H16" s="5" t="inlineStr">
-        <is>
-          <t>OG584V</t>
-        </is>
-      </c>
-      <c r="I16" s="5" t="inlineStr">
-        <is>
-          <t>MANUAL</t>
-        </is>
-      </c>
-      <c r="J16" s="5" t="inlineStr">
-        <is>
-          <t>DANIEL ARAUJO</t>
-        </is>
-      </c>
-      <c r="K16" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="L16" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="M16" s="6" t="n">
-        <v>45828.50416666667</v>
-      </c>
-      <c r="N16" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O16" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P16" s="5" t="inlineStr">
-        <is>
-          <t>OFF LINE</t>
-        </is>
-      </c>
-      <c r="Q16" s="5" t="inlineStr">
-        <is>
-          <t>Invoice</t>
-        </is>
-      </c>
-      <c r="R16" s="5" t="inlineStr">
-        <is>
-          <t>Cartão convênio</t>
-        </is>
-      </c>
-      <c r="S16" s="5" t="inlineStr">
-        <is>
-          <t>Aéreo</t>
-        </is>
-      </c>
-      <c r="T16" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="U16" s="5" t="inlineStr">
-        <is>
-          <t>Grupo Kontrip</t>
-        </is>
-      </c>
-      <c r="V16" s="5" t="inlineStr">
-        <is>
-          <t>Porto de Galinhas Convention e Visitors Bureau</t>
-        </is>
-      </c>
-      <c r="W16" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X16" s="5" t="inlineStr">
-        <is>
-          <t>Azul Linhas Aereas</t>
-        </is>
-      </c>
-      <c r="Y16" s="5" t="n">
-        <v>3023285536</v>
-      </c>
-      <c r="Z16" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AA16" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB16" s="5" t="n">
-        <v>612.54</v>
-      </c>
-      <c r="AC16" s="5" t="n">
-        <v>119.51</v>
-      </c>
-      <c r="AD16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ16" s="5" t="inlineStr">
-        <is>
-          <t>36Faltou informar rateio de centro de custo/projeto abaixo da accounting</t>
-        </is>
-      </c>
-      <c r="AK16" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AL16" s="5" t="inlineStr">
-        <is>
-          <t>Falta de informação Gerencial</t>
-        </is>
-      </c>
-      <c r="AM16" s="5" t="inlineStr">
-        <is>
-          <t>Rateio de centro de custo/projeto</t>
-        </is>
-      </c>
-      <c r="AN16" s="5" t="inlineStr">
-        <is>
-          <t>Dados Gerenciais</t>
-        </is>
-      </c>
-      <c r="AO16" s="5" t="inlineStr">
-        <is>
-          <t>Qualidade dos dados</t>
-        </is>
-      </c>
-      <c r="AP16" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP VIAGENS</t>
-        </is>
-      </c>
-      <c r="AQ16" s="5" t="inlineStr">
         <is>
           <t>Operações - KONTRIP</t>
         </is>

</xml_diff>

<commit_message>
Atualiza filtros e métricas em scripts de integração
Adiciona filtro para excluir resolvidos com mais de 6 meses em '3 - atualizacao_status.py'. Em '4 - envio_relatorios.py', inclui cálculo de porcentagem de vendas integradas e ajusta leitura de relatórios. Atualiza diversos arquivos Excel e PDF
</commit_message>
<xml_diff>
--- a/Integration Quality/EMPRESAS/Relatorio - KONTRIP VIAGENS.xlsx
+++ b/Integration Quality/EMPRESAS/Relatorio - KONTRIP VIAGENS.xlsx
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ14"/>
+  <dimension ref="A1:AQ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,10 +700,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="n">
-        <v>22461262</v>
+        <v>22504723</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>23300940</v>
+        <v>23337436</v>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
@@ -711,24 +711,24 @@
         </is>
       </c>
       <c r="D2" s="6" t="n">
-        <v>45834.70292824074</v>
+        <v>45841.60965277778</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>45834.70704861111</v>
+        <v>45841.61076388889</v>
       </c>
       <c r="F2" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G2" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>GMPQBQ</t>
+          <t>FYJJJU</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="J2" s="5" t="inlineStr">
         <is>
-          <t>DA SILVA CASTRO/VICTOR</t>
+          <t>LUIS CASTRO SCATOLINI/TIAGO</t>
         </is>
       </c>
       <c r="K2" s="5" t="inlineStr">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="M2" s="6" t="n">
-        <v>45834.69861111111</v>
+        <v>45841.60902777778</v>
       </c>
       <c r="N2" s="5" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
       </c>
       <c r="V2" s="5" t="inlineStr">
         <is>
-          <t>Pessoa e Pessoa Advogados Associados</t>
+          <t>Instituto Atlantico</t>
         </is>
       </c>
       <c r="W2" s="5" t="inlineStr">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="Y2" s="5" t="n">
-        <v>2140277329</v>
+        <v>2140681925</v>
       </c>
       <c r="Z2" s="5" t="inlineStr">
         <is>
@@ -823,10 +823,10 @@
         </is>
       </c>
       <c r="AB2" s="5" t="n">
-        <v>1191.9</v>
+        <v>386.79</v>
       </c>
       <c r="AC2" s="5" t="n">
-        <v>104.89</v>
+        <v>400</v>
       </c>
       <c r="AD2" s="5" t="n">
         <v>0</v>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="AH2" s="5" t="n">
-        <v>71.51000000000001</v>
+        <v>40</v>
       </c>
       <c r="AI2" s="5" t="inlineStr">
         <is>
@@ -850,7 +850,7 @@
       </c>
       <c r="AJ2" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo não preenchido! (ACC01)</t>
+          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
         </is>
       </c>
       <c r="AK2" s="5" t="inlineStr">
@@ -860,17 +860,17 @@
       </c>
       <c r="AL2" s="5" t="inlineStr">
         <is>
-          <t>Centro de custo</t>
+          <t>Duplicidade de RLOC</t>
         </is>
       </c>
       <c r="AM2" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Campo RLOC</t>
         </is>
       </c>
       <c r="AN2" s="5" t="inlineStr">
         <is>
-          <t>Dados do Fornecedor</t>
+          <t>Duplicidade de Contabilização</t>
         </is>
       </c>
       <c r="AO2" s="5" t="inlineStr">
@@ -891,59 +891,59 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="n">
-        <v>22459992</v>
+        <v>22504763</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>23299710</v>
+        <v>23337473</v>
       </c>
       <c r="C3" s="5" t="inlineStr">
         <is>
-          <t>ACC</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D3" s="6" t="n">
-        <v>45834.52964120371</v>
+        <v>45841.61942129629</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>45834.73059027778</v>
+        <v>45841.62157407407</v>
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G3" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>LA9571600AUXS</t>
+          <t>FXXJWY</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J3" s="5" t="inlineStr">
         <is>
-          <t>VALERIA GOMES LEAL</t>
+          <t>LUIS CASTRO SCATOLINI/TIAGO</t>
         </is>
       </c>
       <c r="K3" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L3" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M3" s="6" t="n">
-        <v>45833.52916666667</v>
+        <v>45841.61875</v>
       </c>
       <c r="N3" s="5" t="inlineStr">
         <is>
@@ -962,12 +962,12 @@
       </c>
       <c r="Q3" s="5" t="inlineStr">
         <is>
-          <t>Invoice</t>
+          <t>Cartão de crédito</t>
         </is>
       </c>
       <c r="R3" s="5" t="inlineStr">
         <is>
-          <t>Cartão convênio</t>
+          <t>Cartão de crédito</t>
         </is>
       </c>
       <c r="S3" s="5" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="V3" s="5" t="inlineStr">
         <is>
-          <t>Kontrip - Vendas Cartao de Credito</t>
+          <t>Instituto Atlantico</t>
         </is>
       </c>
       <c r="W3" s="5" t="inlineStr">
@@ -997,11 +997,11 @@
       </c>
       <c r="X3" s="5" t="inlineStr">
         <is>
-          <t>Latam Airlines Brasil</t>
+          <t>Gol Linhas Aereas</t>
         </is>
       </c>
       <c r="Y3" s="5" t="n">
-        <v>2238480836</v>
+        <v>2140683530</v>
       </c>
       <c r="Z3" s="5" t="inlineStr">
         <is>
@@ -1014,10 +1014,10 @@
         </is>
       </c>
       <c r="AB3" s="5" t="n">
-        <v>1785.44</v>
+        <v>595.79</v>
       </c>
       <c r="AC3" s="5" t="n">
-        <v>78.38</v>
+        <v>40</v>
       </c>
       <c r="AD3" s="5" t="n">
         <v>0</v>
@@ -1032,16 +1032,16 @@
         <v>0</v>
       </c>
       <c r="AH3" s="5" t="n">
-        <v>30.53</v>
+        <v>400</v>
       </c>
       <c r="AI3" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ3" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
         </is>
       </c>
       <c r="AK3" s="5" t="inlineStr">
@@ -1051,17 +1051,17 @@
       </c>
       <c r="AL3" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Duplicidade de RLOC</t>
         </is>
       </c>
       <c r="AM3" s="5" t="inlineStr">
         <is>
-          <t>Rateio de centro de custo/projeto</t>
+          <t>Campo RLOC</t>
         </is>
       </c>
       <c r="AN3" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Duplicidade de Contabilização</t>
         </is>
       </c>
       <c r="AO3" s="5" t="inlineStr">
@@ -1082,59 +1082,59 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="n">
-        <v>22460028</v>
+        <v>22505709</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>23299735</v>
+        <v>23338405</v>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>ACC</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D4" s="6" t="n">
-        <v>45834.53344907407</v>
+        <v>45841.73232638889</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>45834.73065972222</v>
+        <v>45841.73412037037</v>
       </c>
       <c r="F4" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G4" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
-          <t>LA9577150CBWZ</t>
+          <t>LA9575803BKIN</t>
         </is>
       </c>
       <c r="I4" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J4" s="5" t="inlineStr">
         <is>
-          <t>FRANCISCO CANINDE FERNANDES JUNIOR</t>
+          <t>SANTANA PEREIRA/ANDERSON</t>
         </is>
       </c>
       <c r="K4" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L4" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M4" s="6" t="n">
-        <v>45833.53333333333</v>
+        <v>45841.725</v>
       </c>
       <c r="N4" s="5" t="inlineStr">
         <is>
@@ -1173,12 +1173,12 @@
       </c>
       <c r="U4" s="5" t="inlineStr">
         <is>
-          <t>Grupo Kontrip</t>
+          <t>Grupo Sacs</t>
         </is>
       </c>
       <c r="V4" s="5" t="inlineStr">
         <is>
-          <t>Nossa Engenharia e Servicos</t>
+          <t>Sacs Construcao e Montagem Ltda</t>
         </is>
       </c>
       <c r="W4" s="5" t="inlineStr">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="Y4" s="5" t="n">
-        <v>2238555012</v>
+        <v>2239671708</v>
       </c>
       <c r="Z4" s="5" t="inlineStr">
         <is>
@@ -1205,10 +1205,10 @@
         </is>
       </c>
       <c r="AB4" s="5" t="n">
-        <v>1199.69</v>
+        <v>1660.33</v>
       </c>
       <c r="AC4" s="5" t="n">
-        <v>102.22</v>
+        <v>44.27</v>
       </c>
       <c r="AD4" s="5" t="n">
         <v>0</v>
@@ -1223,16 +1223,16 @@
         <v>0</v>
       </c>
       <c r="AH4" s="5" t="n">
-        <v>20.51</v>
+        <v>73.79000000000001</v>
       </c>
       <c r="AI4" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ4" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>o. Valor Líquido: 1.606,45 Débitos: 36,64 Créditos: 1.704,60. Saldo: -61,51 Saldo percentual: 3,83</t>
         </is>
       </c>
       <c r="AK4" s="5" t="inlineStr">
@@ -1242,17 +1242,17 @@
       </c>
       <c r="AL4" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Não identificado</t>
         </is>
       </c>
       <c r="AM4" s="5" t="inlineStr">
         <is>
-          <t>Rateio de centro de custo/projeto</t>
+          <t>Análise Benner</t>
         </is>
       </c>
       <c r="AN4" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Sistema</t>
         </is>
       </c>
       <c r="AO4" s="5" t="inlineStr">
@@ -1273,59 +1273,59 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="n">
-        <v>22459944</v>
+        <v>22505709</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>23299686</v>
+        <v>23338406</v>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
-          <t>ACC</t>
+          <t>ACC02</t>
         </is>
       </c>
       <c r="D5" s="6" t="n">
-        <v>45834.52306712963</v>
+        <v>45841.73232638889</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>45834.73011574074</v>
+        <v>45841.73412037037</v>
       </c>
       <c r="F5" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G5" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
-          <t>LA9572362DNZW</t>
+          <t>LA9575803BKIN</t>
         </is>
       </c>
       <c r="I5" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J5" s="5" t="inlineStr">
         <is>
-          <t>CAIO FABIO ALVES CASTRO</t>
+          <t>DA CONCEIÇÃO SANTOS BARRETO/VALTER</t>
         </is>
       </c>
       <c r="K5" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L5" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M5" s="6" t="n">
-        <v>45833.52291666667</v>
+        <v>45841.725</v>
       </c>
       <c r="N5" s="5" t="inlineStr">
         <is>
@@ -1364,12 +1364,12 @@
       </c>
       <c r="U5" s="5" t="inlineStr">
         <is>
-          <t>Grupo Kontrip</t>
+          <t>Grupo Sacs</t>
         </is>
       </c>
       <c r="V5" s="5" t="inlineStr">
         <is>
-          <t>Marques e Bezerra Ltda</t>
+          <t>Sacs Construcao e Montagem Ltda</t>
         </is>
       </c>
       <c r="W5" s="5" t="inlineStr">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="Y5" s="5" t="n">
-        <v>2238457649</v>
+        <v>2239671709</v>
       </c>
       <c r="Z5" s="5" t="inlineStr">
         <is>
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="AB5" s="5" t="n">
-        <v>1608.04</v>
+        <v>1660.33</v>
       </c>
       <c r="AC5" s="5" t="n">
-        <v>95.34</v>
+        <v>44.27</v>
       </c>
       <c r="AD5" s="5" t="n">
         <v>0</v>
@@ -1414,16 +1414,16 @@
         <v>0</v>
       </c>
       <c r="AH5" s="5" t="n">
-        <v>27.5</v>
+        <v>0</v>
       </c>
       <c r="AI5" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ5" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>o. Valor Líquido: 1.606,45 Débitos: 36,64 Créditos: 1.704,60. Saldo: -61,51 Saldo percentual: 3,83</t>
         </is>
       </c>
       <c r="AK5" s="5" t="inlineStr">
@@ -1433,17 +1433,17 @@
       </c>
       <c r="AL5" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Não identificado</t>
         </is>
       </c>
       <c r="AM5" s="5" t="inlineStr">
         <is>
-          <t>Rateio de centro de custo/projeto</t>
+          <t>Análise Benner</t>
         </is>
       </c>
       <c r="AN5" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Sistema</t>
         </is>
       </c>
       <c r="AO5" s="5" t="inlineStr">
@@ -1464,59 +1464,59 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="n">
-        <v>22459872</v>
+        <v>22505709</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>23299568</v>
+        <v>23338407</v>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC03</t>
         </is>
       </c>
       <c r="D6" s="6" t="n">
-        <v>45834.51140046296</v>
+        <v>45841.73232638889</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>45834.72637731482</v>
+        <v>45841.73412037037</v>
       </c>
       <c r="F6" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G6" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
-          <t>SF3F6L</t>
+          <t>LA9575803BKIN</t>
         </is>
       </c>
       <c r="I6" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J6" s="5" t="inlineStr">
         <is>
-          <t>CAMILA DO NASCIMENTO CAMPOS KAERCHER</t>
+          <t>ALVES PIRES/FABIO</t>
         </is>
       </c>
       <c r="K6" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L6" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M6" s="6" t="n">
-        <v>45833.51111111111</v>
+        <v>45841.725</v>
       </c>
       <c r="N6" s="5" t="inlineStr">
         <is>
@@ -1535,12 +1535,12 @@
       </c>
       <c r="Q6" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Invoice</t>
         </is>
       </c>
       <c r="R6" s="5" t="inlineStr">
         <is>
-          <t>Cartão de crédito</t>
+          <t>Cartão convênio</t>
         </is>
       </c>
       <c r="S6" s="5" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="U6" s="5" t="inlineStr">
         <is>
-          <t>Grupo Kontrip</t>
+          <t>Grupo Sacs</t>
         </is>
       </c>
       <c r="V6" s="5" t="inlineStr">
         <is>
-          <t>Kaercher Treinamentos</t>
+          <t>Sacs Construcao e Montagem Ltda</t>
         </is>
       </c>
       <c r="W6" s="5" t="inlineStr">
@@ -1570,11 +1570,11 @@
       </c>
       <c r="X6" s="5" t="inlineStr">
         <is>
-          <t>Azul Linhas Aereas</t>
+          <t>Latam Airlines Brasil</t>
         </is>
       </c>
       <c r="Y6" s="5" t="n">
-        <v>3023299567</v>
+        <v>2239671710</v>
       </c>
       <c r="Z6" s="5" t="inlineStr">
         <is>
@@ -1587,10 +1587,10 @@
         </is>
       </c>
       <c r="AB6" s="5" t="n">
-        <v>1751.51</v>
+        <v>1660.33</v>
       </c>
       <c r="AC6" s="5" t="n">
-        <v>74.59</v>
+        <v>44.27</v>
       </c>
       <c r="AD6" s="5" t="n">
         <v>0</v>
@@ -1605,16 +1605,16 @@
         <v>0</v>
       </c>
       <c r="AH6" s="5" t="n">
-        <v>472.91</v>
+        <v>0</v>
       </c>
       <c r="AI6" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ6" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>o. Valor Líquido: 1.606,45 Débitos: 36,64 Créditos: 1.704,60. Saldo: -61,51 Saldo percentual: 3,83</t>
         </is>
       </c>
       <c r="AK6" s="5" t="inlineStr">
@@ -1624,17 +1624,17 @@
       </c>
       <c r="AL6" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Não identificado</t>
         </is>
       </c>
       <c r="AM6" s="5" t="inlineStr">
         <is>
-          <t>Rateio de centro de custo/projeto</t>
+          <t>Análise Benner</t>
         </is>
       </c>
       <c r="AN6" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Sistema</t>
         </is>
       </c>
       <c r="AO6" s="5" t="inlineStr">
@@ -1655,59 +1655,59 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="n">
-        <v>22459872</v>
+        <v>22507127</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>23299589</v>
+        <v>23339842</v>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>ACC02</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D7" s="6" t="n">
-        <v>45834.51140046296</v>
+        <v>45841.81936342592</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>45834.72637731482</v>
+        <v>45841.82116898148</v>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
-          <t>SF3F6L</t>
+          <t>OQE2WX</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
-          <t>MARIANA CERQUEIRA DE ALMEIDA</t>
+          <t>de Sousa Teixeira/Janai</t>
         </is>
       </c>
       <c r="K7" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L7" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M7" s="6" t="n">
-        <v>45833.51111111111</v>
+        <v>45841.81805555556</v>
       </c>
       <c r="N7" s="5" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="V7" s="5" t="inlineStr">
         <is>
-          <t>Kaercher Treinamentos</t>
+          <t>Atakarejo Distribuidor de Alimentos e Bebidas Eireli</t>
         </is>
       </c>
       <c r="W7" s="5" t="inlineStr">
@@ -1765,7 +1765,7 @@
         </is>
       </c>
       <c r="Y7" s="5" t="n">
-        <v>3023299591</v>
+        <v>575077156</v>
       </c>
       <c r="Z7" s="5" t="inlineStr">
         <is>
@@ -1778,10 +1778,10 @@
         </is>
       </c>
       <c r="AB7" s="5" t="n">
-        <v>1751.51</v>
+        <v>404.5</v>
       </c>
       <c r="AC7" s="5" t="n">
-        <v>74.59</v>
+        <v>450</v>
       </c>
       <c r="AD7" s="5" t="n">
         <v>0</v>
@@ -1796,16 +1796,16 @@
         <v>0</v>
       </c>
       <c r="AH7" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AI7" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ7" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
         </is>
       </c>
       <c r="AK7" s="5" t="inlineStr">
@@ -1815,17 +1815,17 @@
       </c>
       <c r="AL7" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Duplicidade de RLOC</t>
         </is>
       </c>
       <c r="AM7" s="5" t="inlineStr">
         <is>
-          <t>Rateio de centro de custo/projeto</t>
+          <t>Campo RLOC</t>
         </is>
       </c>
       <c r="AN7" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Duplicidade de Contabilização</t>
         </is>
       </c>
       <c r="AO7" s="5" t="inlineStr">
@@ -1846,35 +1846,35 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="n">
-        <v>22459872</v>
+        <v>22505034</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>23299595</v>
+        <v>23337766</v>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>ACC03</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D8" s="6" t="n">
-        <v>45834.51140046296</v>
+        <v>45841.65449074074</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>45834.72637731482</v>
+        <v>45841.6600462963</v>
       </c>
       <c r="F8" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G8" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H8" s="5" t="inlineStr">
         <is>
-          <t>SF3F6L</t>
+          <t>WLJNWZ</t>
         </is>
       </c>
       <c r="I8" s="5" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="J8" s="5" t="inlineStr">
         <is>
-          <t>LUCAS GONCALVES GOMES SILVA</t>
+          <t>FERNANDO TAVARES DA SILVA</t>
         </is>
       </c>
       <c r="K8" s="5" t="inlineStr">
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="M8" s="6" t="n">
-        <v>45833.51111111111</v>
+        <v>45840.65416666667</v>
       </c>
       <c r="N8" s="5" t="inlineStr">
         <is>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="V8" s="5" t="inlineStr">
         <is>
-          <t>Kaercher Treinamentos</t>
+          <t>Mauro Goncalve Antonelli</t>
         </is>
       </c>
       <c r="W8" s="5" t="inlineStr">
@@ -1956,7 +1956,7 @@
         </is>
       </c>
       <c r="Y8" s="5" t="n">
-        <v>3023299596</v>
+        <v>3023337765</v>
       </c>
       <c r="Z8" s="5" t="inlineStr">
         <is>
@@ -1969,10 +1969,10 @@
         </is>
       </c>
       <c r="AB8" s="5" t="n">
-        <v>1751.51</v>
+        <v>1017.8</v>
       </c>
       <c r="AC8" s="5" t="n">
-        <v>74.59</v>
+        <v>107.34</v>
       </c>
       <c r="AD8" s="5" t="n">
         <v>0</v>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="AH8" s="5" t="n">
-        <v>0</v>
+        <v>274.81</v>
       </c>
       <c r="AI8" s="5" t="inlineStr">
         <is>
@@ -2037,59 +2037,59 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="n">
-        <v>22459937</v>
+        <v>22505034</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>23299646</v>
+        <v>23337772</v>
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC02</t>
         </is>
       </c>
       <c r="D9" s="6" t="n">
-        <v>45834.52216435185</v>
+        <v>45841.65449074074</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>45834.52375</v>
+        <v>45841.6600462963</v>
       </c>
       <c r="F9" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G9" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H9" s="5" t="inlineStr">
         <is>
-          <t>XNRYUD</t>
+          <t>WLJNWZ</t>
         </is>
       </c>
       <c r="I9" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J9" s="5" t="inlineStr">
         <is>
-          <t>DE ARRUDA QUINTEIRO/BRUNNA</t>
+          <t>RUDINEI GODOY</t>
         </is>
       </c>
       <c r="K9" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L9" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M9" s="6" t="n">
-        <v>45834.52152777778</v>
+        <v>45840.65416666667</v>
       </c>
       <c r="N9" s="5" t="inlineStr">
         <is>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="V9" s="5" t="inlineStr">
         <is>
-          <t>Kontrip - Vendas Cartao de Credito</t>
+          <t>Mauro Goncalve Antonelli</t>
         </is>
       </c>
       <c r="W9" s="5" t="inlineStr">
@@ -2147,7 +2147,7 @@
         </is>
       </c>
       <c r="Y9" s="5" t="n">
-        <v>496701246</v>
+        <v>3023337775</v>
       </c>
       <c r="Z9" s="5" t="inlineStr">
         <is>
@@ -2160,10 +2160,10 @@
         </is>
       </c>
       <c r="AB9" s="5" t="n">
-        <v>2089.19</v>
+        <v>1017.8</v>
       </c>
       <c r="AC9" s="5" t="n">
-        <v>450</v>
+        <v>107.34</v>
       </c>
       <c r="AD9" s="5" t="n">
         <v>0</v>
@@ -2178,16 +2178,16 @@
         <v>0</v>
       </c>
       <c r="AH9" s="5" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ9" s="5" t="inlineStr">
         <is>
-          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK9" s="5" t="inlineStr">
@@ -2197,17 +2197,17 @@
       </c>
       <c r="AL9" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de RLOC</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM9" s="5" t="inlineStr">
         <is>
-          <t>Campo RLOC</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN9" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO9" s="5" t="inlineStr">
@@ -2228,59 +2228,59 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="n">
-        <v>22461196</v>
+        <v>22505034</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>23300868</v>
+        <v>23337777</v>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>ACC01</t>
+          <t>ACC03</t>
         </is>
       </c>
       <c r="D10" s="6" t="n">
-        <v>45834.69434027778</v>
+        <v>45841.65449074074</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>45834.69774305556</v>
+        <v>45841.6600462963</v>
       </c>
       <c r="F10" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G10" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H10" s="5" t="inlineStr">
         <is>
-          <t>NJZS5M</t>
+          <t>WLJNWZ</t>
         </is>
       </c>
       <c r="I10" s="5" t="inlineStr">
         <is>
-          <t>EBOOKING</t>
+          <t>MANUAL</t>
         </is>
       </c>
       <c r="J10" s="5" t="inlineStr">
         <is>
-          <t>Varalda/Adriana</t>
+          <t>JOAO AUGUSTO</t>
         </is>
       </c>
       <c r="K10" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="L10" s="5" t="inlineStr">
         <is>
-          <t>Kontrip</t>
+          <t>Juliana Cardoso</t>
         </is>
       </c>
       <c r="M10" s="6" t="n">
-        <v>45834.67777777778</v>
+        <v>45840.65416666667</v>
       </c>
       <c r="N10" s="5" t="inlineStr">
         <is>
@@ -2324,7 +2324,7 @@
       </c>
       <c r="V10" s="5" t="inlineStr">
         <is>
-          <t>Kontrip - Vendas Cartao de Credito</t>
+          <t>Mauro Goncalve Antonelli</t>
         </is>
       </c>
       <c r="W10" s="5" t="inlineStr">
@@ -2338,7 +2338,7 @@
         </is>
       </c>
       <c r="Y10" s="5" t="n">
-        <v>119583055</v>
+        <v>3023337779</v>
       </c>
       <c r="Z10" s="5" t="inlineStr">
         <is>
@@ -2351,10 +2351,10 @@
         </is>
       </c>
       <c r="AB10" s="5" t="n">
-        <v>1790</v>
+        <v>1017.8</v>
       </c>
       <c r="AC10" s="5" t="n">
-        <v>0</v>
+        <v>107.34</v>
       </c>
       <c r="AD10" s="5" t="n">
         <v>0</v>
@@ -2369,16 +2369,16 @@
         <v>0</v>
       </c>
       <c r="AH10" s="5" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="5" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>-</t>
         </is>
       </c>
       <c r="AJ10" s="5" t="inlineStr">
         <is>
-          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
+          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
         </is>
       </c>
       <c r="AK10" s="5" t="inlineStr">
@@ -2388,17 +2388,17 @@
       </c>
       <c r="AL10" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de RLOC</t>
+          <t>Falta de informação Gerencial</t>
         </is>
       </c>
       <c r="AM10" s="5" t="inlineStr">
         <is>
-          <t>Campo RLOC</t>
+          <t>Rateio de centro de custo/projeto</t>
         </is>
       </c>
       <c r="AN10" s="5" t="inlineStr">
         <is>
-          <t>Duplicidade de Contabilização</t>
+          <t>Dados Gerenciais</t>
         </is>
       </c>
       <c r="AO10" s="5" t="inlineStr">
@@ -2419,59 +2419,59 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="n">
-        <v>22459821</v>
+        <v>22505228</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>23299526</v>
+        <v>23337948</v>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>ACC</t>
+          <t>ACC01</t>
         </is>
       </c>
       <c r="D11" s="6" t="n">
-        <v>45834.50327546296</v>
+        <v>45841.67219907408</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>45834.70680555556</v>
+        <v>45841.67327546296</v>
       </c>
       <c r="F11" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="G11" s="5" t="inlineStr">
         <is>
-          <t>03 a 05 dias</t>
+          <t>0 a 02 dias</t>
         </is>
       </c>
       <c r="H11" s="5" t="inlineStr">
         <is>
-          <t>RK8PPM</t>
+          <t>IMQ8ND</t>
         </is>
       </c>
       <c r="I11" s="5" t="inlineStr">
         <is>
-          <t>MANUAL</t>
+          <t>EBOOKING</t>
         </is>
       </c>
       <c r="J11" s="5" t="inlineStr">
         <is>
-          <t>THIAGO DE LIMA FAUSTINO</t>
+          <t>SILVA/GIVANILDO</t>
         </is>
       </c>
       <c r="K11" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="L11" s="5" t="inlineStr">
         <is>
-          <t>Juliana Cardoso</t>
+          <t>Kontrip</t>
         </is>
       </c>
       <c r="M11" s="6" t="n">
-        <v>45833.50277777778</v>
+        <v>45841.67013888889</v>
       </c>
       <c r="N11" s="5" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="V11" s="5" t="inlineStr">
         <is>
-          <t>Kontrip - Vendas Cartao de Credito</t>
+          <t>Topocart Topografia Engenharia e Aerolevantamentos</t>
         </is>
       </c>
       <c r="W11" s="5" t="inlineStr">
@@ -2529,7 +2529,7 @@
         </is>
       </c>
       <c r="Y11" s="5" t="n">
-        <v>3023299525</v>
+        <v>423506088</v>
       </c>
       <c r="Z11" s="5" t="inlineStr">
         <is>
@@ -2542,10 +2542,10 @@
         </is>
       </c>
       <c r="AB11" s="5" t="n">
-        <v>1058.92</v>
+        <v>226.64</v>
       </c>
       <c r="AC11" s="5" t="n">
-        <v>34.11</v>
+        <v>900</v>
       </c>
       <c r="AD11" s="5" t="n">
         <v>0</v>
@@ -2560,16 +2560,16 @@
         <v>0</v>
       </c>
       <c r="AH11" s="5" t="n">
-        <v>95.3</v>
+        <v>40</v>
       </c>
       <c r="AI11" s="5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="AJ11" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
+          <t>Pnr já existente. A duplicidade de rloc é permitida apenas 6 meses após o último pnr emitido</t>
         </is>
       </c>
       <c r="AK11" s="5" t="inlineStr">
@@ -2579,17 +2579,17 @@
       </c>
       <c r="AL11" s="5" t="inlineStr">
         <is>
-          <t>Falta de informação Gerencial</t>
+          <t>Duplicidade de RLOC</t>
         </is>
       </c>
       <c r="AM11" s="5" t="inlineStr">
         <is>
-          <t>Rateio de centro de custo/projeto</t>
+          <t>Campo RLOC</t>
         </is>
       </c>
       <c r="AN11" s="5" t="inlineStr">
         <is>
-          <t>Dados Gerenciais</t>
+          <t>Duplicidade de Contabilização</t>
         </is>
       </c>
       <c r="AO11" s="5" t="inlineStr">
@@ -2603,579 +2603,6 @@
         </is>
       </c>
       <c r="AQ11" s="5" t="inlineStr">
-        <is>
-          <t>Operações - KONTRIP</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="n">
-        <v>22460105</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>23299810</v>
-      </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>45834.54712962963</v>
-      </c>
-      <c r="E12" s="6" t="n">
-        <v>45834.72902777778</v>
-      </c>
-      <c r="F12" s="5" t="inlineStr">
-        <is>
-          <t>03 a 05 dias</t>
-        </is>
-      </c>
-      <c r="G12" s="5" t="inlineStr">
-        <is>
-          <t>03 a 05 dias</t>
-        </is>
-      </c>
-      <c r="H12" s="5" t="inlineStr">
-        <is>
-          <t>JHS6PS</t>
-        </is>
-      </c>
-      <c r="I12" s="5" t="inlineStr">
-        <is>
-          <t>MANUAL</t>
-        </is>
-      </c>
-      <c r="J12" s="5" t="inlineStr">
-        <is>
-          <t>CAROLINE CELLI</t>
-        </is>
-      </c>
-      <c r="K12" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="L12" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="M12" s="6" t="n">
-        <v>45833.54652777778</v>
-      </c>
-      <c r="N12" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O12" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P12" s="5" t="inlineStr">
-        <is>
-          <t>OFF LINE</t>
-        </is>
-      </c>
-      <c r="Q12" s="5" t="inlineStr">
-        <is>
-          <t>Cartão de crédito</t>
-        </is>
-      </c>
-      <c r="R12" s="5" t="inlineStr">
-        <is>
-          <t>Cartão de crédito</t>
-        </is>
-      </c>
-      <c r="S12" s="5" t="inlineStr">
-        <is>
-          <t>Aéreo</t>
-        </is>
-      </c>
-      <c r="T12" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="U12" s="5" t="inlineStr">
-        <is>
-          <t>Grupo Kontrip</t>
-        </is>
-      </c>
-      <c r="V12" s="5" t="inlineStr">
-        <is>
-          <t>Mauro Goncalve Antonelli</t>
-        </is>
-      </c>
-      <c r="W12" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X12" s="5" t="inlineStr">
-        <is>
-          <t>Azul Linhas Aereas</t>
-        </is>
-      </c>
-      <c r="Y12" s="5" t="n">
-        <v>3023299809</v>
-      </c>
-      <c r="Z12" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AA12" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB12" s="5" t="n">
-        <v>1574.88</v>
-      </c>
-      <c r="AC12" s="5" t="n">
-        <v>46.72</v>
-      </c>
-      <c r="AD12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="5" t="n">
-        <v>141.74</v>
-      </c>
-      <c r="AI12" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ12" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
-        </is>
-      </c>
-      <c r="AK12" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AL12" s="5" t="inlineStr">
-        <is>
-          <t>Falta de informação Gerencial</t>
-        </is>
-      </c>
-      <c r="AM12" s="5" t="inlineStr">
-        <is>
-          <t>Rateio de centro de custo/projeto</t>
-        </is>
-      </c>
-      <c r="AN12" s="5" t="inlineStr">
-        <is>
-          <t>Dados Gerenciais</t>
-        </is>
-      </c>
-      <c r="AO12" s="5" t="inlineStr">
-        <is>
-          <t>Qualidade dos dados</t>
-        </is>
-      </c>
-      <c r="AP12" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP VIAGENS</t>
-        </is>
-      </c>
-      <c r="AQ12" s="5" t="inlineStr">
-        <is>
-          <t>Operações - KONTRIP</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="n">
-        <v>22459766</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>23299457</v>
-      </c>
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>45834.49883101852</v>
-      </c>
-      <c r="E13" s="6" t="n">
-        <v>45834.70751157407</v>
-      </c>
-      <c r="F13" s="5" t="inlineStr">
-        <is>
-          <t>03 a 05 dias</t>
-        </is>
-      </c>
-      <c r="G13" s="5" t="inlineStr">
-        <is>
-          <t>03 a 05 dias</t>
-        </is>
-      </c>
-      <c r="H13" s="5" t="inlineStr">
-        <is>
-          <t>GRS1HB</t>
-        </is>
-      </c>
-      <c r="I13" s="5" t="inlineStr">
-        <is>
-          <t>MANUAL</t>
-        </is>
-      </c>
-      <c r="J13" s="5" t="inlineStr">
-        <is>
-          <t>SAMUEL SILVA</t>
-        </is>
-      </c>
-      <c r="K13" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="L13" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="M13" s="6" t="n">
-        <v>45833.49861111111</v>
-      </c>
-      <c r="N13" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O13" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P13" s="5" t="inlineStr">
-        <is>
-          <t>OFF LINE</t>
-        </is>
-      </c>
-      <c r="Q13" s="5" t="inlineStr">
-        <is>
-          <t>Cartão de crédito</t>
-        </is>
-      </c>
-      <c r="R13" s="5" t="inlineStr">
-        <is>
-          <t>Cartão de crédito</t>
-        </is>
-      </c>
-      <c r="S13" s="5" t="inlineStr">
-        <is>
-          <t>Aéreo</t>
-        </is>
-      </c>
-      <c r="T13" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="U13" s="5" t="inlineStr">
-        <is>
-          <t>Grupo Kontrip</t>
-        </is>
-      </c>
-      <c r="V13" s="5" t="inlineStr">
-        <is>
-          <t>Galzer Importacao e Exportacao Ltda</t>
-        </is>
-      </c>
-      <c r="W13" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X13" s="5" t="inlineStr">
-        <is>
-          <t>Azul Linhas Aereas</t>
-        </is>
-      </c>
-      <c r="Y13" s="5" t="n">
-        <v>3023299456</v>
-      </c>
-      <c r="Z13" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AA13" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB13" s="5" t="n">
-        <v>227.84</v>
-      </c>
-      <c r="AC13" s="5" t="n">
-        <v>65</v>
-      </c>
-      <c r="AD13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="5" t="n">
-        <v>20.51</v>
-      </c>
-      <c r="AI13" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ13" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
-        </is>
-      </c>
-      <c r="AK13" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AL13" s="5" t="inlineStr">
-        <is>
-          <t>Falta de informação Gerencial</t>
-        </is>
-      </c>
-      <c r="AM13" s="5" t="inlineStr">
-        <is>
-          <t>Rateio de centro de custo/projeto</t>
-        </is>
-      </c>
-      <c r="AN13" s="5" t="inlineStr">
-        <is>
-          <t>Dados Gerenciais</t>
-        </is>
-      </c>
-      <c r="AO13" s="5" t="inlineStr">
-        <is>
-          <t>Qualidade dos dados</t>
-        </is>
-      </c>
-      <c r="AP13" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP VIAGENS</t>
-        </is>
-      </c>
-      <c r="AQ13" s="5" t="inlineStr">
-        <is>
-          <t>Operações - KONTRIP</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="n">
-        <v>22459866</v>
-      </c>
-      <c r="B14" s="5" t="n">
-        <v>23299554</v>
-      </c>
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>ACC</t>
-        </is>
-      </c>
-      <c r="D14" s="6" t="n">
-        <v>45834.50763888889</v>
-      </c>
-      <c r="E14" s="6" t="n">
-        <v>45834.72603009259</v>
-      </c>
-      <c r="F14" s="5" t="inlineStr">
-        <is>
-          <t>03 a 05 dias</t>
-        </is>
-      </c>
-      <c r="G14" s="5" t="inlineStr">
-        <is>
-          <t>03 a 05 dias</t>
-        </is>
-      </c>
-      <c r="H14" s="5" t="inlineStr">
-        <is>
-          <t>GLBGMG</t>
-        </is>
-      </c>
-      <c r="I14" s="5" t="inlineStr">
-        <is>
-          <t>MANUAL</t>
-        </is>
-      </c>
-      <c r="J14" s="5" t="inlineStr">
-        <is>
-          <t>CHARLLES RODRIGUES</t>
-        </is>
-      </c>
-      <c r="K14" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="L14" s="5" t="inlineStr">
-        <is>
-          <t>Juliana Cardoso</t>
-        </is>
-      </c>
-      <c r="M14" s="6" t="n">
-        <v>45833.50763888889</v>
-      </c>
-      <c r="N14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P14" s="5" t="inlineStr">
-        <is>
-          <t>OFF LINE</t>
-        </is>
-      </c>
-      <c r="Q14" s="5" t="inlineStr">
-        <is>
-          <t>Cartão de crédito</t>
-        </is>
-      </c>
-      <c r="R14" s="5" t="inlineStr">
-        <is>
-          <t>Cartão de crédito</t>
-        </is>
-      </c>
-      <c r="S14" s="5" t="inlineStr">
-        <is>
-          <t>Aéreo</t>
-        </is>
-      </c>
-      <c r="T14" s="5" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="U14" s="5" t="inlineStr">
-        <is>
-          <t>Grupo Kontrip</t>
-        </is>
-      </c>
-      <c r="V14" s="5" t="inlineStr">
-        <is>
-          <t>Galzer Importacao e Exportacao Ltda</t>
-        </is>
-      </c>
-      <c r="W14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X14" s="5" t="inlineStr">
-        <is>
-          <t>Azul Linhas Aereas</t>
-        </is>
-      </c>
-      <c r="Y14" s="5" t="n">
-        <v>3023299553</v>
-      </c>
-      <c r="Z14" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AA14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB14" s="5" t="n">
-        <v>232.34</v>
-      </c>
-      <c r="AC14" s="5" t="n">
-        <v>65</v>
-      </c>
-      <c r="AD14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="5" t="n">
-        <v>20.91</v>
-      </c>
-      <c r="AI14" s="5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AJ14" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">35Ocorreu a seguinte exceção ao gerar a ordem de venda: Ocorreu a seguinte exceção ao inserir o item da ordem de venda:  Faltou informar rateio de </t>
-        </is>
-      </c>
-      <c r="AK14" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP</t>
-        </is>
-      </c>
-      <c r="AL14" s="5" t="inlineStr">
-        <is>
-          <t>Falta de informação Gerencial</t>
-        </is>
-      </c>
-      <c r="AM14" s="5" t="inlineStr">
-        <is>
-          <t>Rateio de centro de custo/projeto</t>
-        </is>
-      </c>
-      <c r="AN14" s="5" t="inlineStr">
-        <is>
-          <t>Dados Gerenciais</t>
-        </is>
-      </c>
-      <c r="AO14" s="5" t="inlineStr">
-        <is>
-          <t>Qualidade dos dados</t>
-        </is>
-      </c>
-      <c r="AP14" s="5" t="inlineStr">
-        <is>
-          <t>KONTRIP VIAGENS</t>
-        </is>
-      </c>
-      <c r="AQ14" s="5" t="inlineStr">
         <is>
           <t>Operações - KONTRIP</t>
         </is>

</xml_diff>